<commit_message>
korekta wyników o przypadkowe zera w algorytmie
</commit_message>
<xml_diff>
--- a/5/1/res/res.xlsx
+++ b/5/1/res/res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartor\IdeaProjects\aisd\5\1\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B2B1A8-159D-4C05-9E10-EE7C37C518E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794923AE-32C6-4F4E-A7F7-7BA079FAB6C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19F8498E-A82F-437B-BA89-2E45E85CD9B8}"/>
+    <workbookView xWindow="-22860" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{19F8498E-A82F-437B-BA89-2E45E85CD9B8}"/>
   </bookViews>
   <sheets>
     <sheet name="ford" sheetId="2" r:id="rId1"/>
@@ -56,9 +56,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,20 +86,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -286,6 +279,22 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -350,43 +359,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.86</c:v>
+                  <c:v>1.439999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2199990000000001</c:v>
+                  <c:v>3.919997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.55</c:v>
+                  <c:v>8.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.339995999999999</c:v>
+                  <c:v>23.789999000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.540000999999997</c:v>
+                  <c:v>67.049994999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158.29997299999999</c:v>
+                  <c:v>170.37994399999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>385.94003300000003</c:v>
+                  <c:v>398.43994099999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>886.61987299999998</c:v>
+                  <c:v>932.16009499999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2025.2098390000001</c:v>
+                  <c:v>2104.0402829999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4485.5703130000002</c:v>
+                  <c:v>4477.7304690000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10279.320313</c:v>
+                  <c:v>10384.141602</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22137.626952999999</c:v>
+                  <c:v>22621.693359000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47450.015625</c:v>
+                  <c:v>48435.164062999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>105516.484375</c:v>
@@ -827,6 +836,23 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -888,7 +914,7 @@
             <c:numRef>
               <c:f>ford!$C$2:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -906,28 +932,28 @@
                   <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0000000000000002E-5</c:v>
+                  <c:v>3.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4999999999999999E-4</c:v>
+                  <c:v>1.3999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1999999999999995E-4</c:v>
+                  <c:v>5.4000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.92E-3</c:v>
+                  <c:v>1.97E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1399999999999996E-3</c:v>
+                  <c:v>6.2100000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5909999999999999E-2</c:v>
+                  <c:v>2.3699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.2580000000000001E-2</c:v>
+                  <c:v>7.8329999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.28611999999999999</c:v>
+                  <c:v>0.27796999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.93942999999999999</c:v>
@@ -1132,7 +1158,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1368,6 +1394,23 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -1432,43 +1475,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.99999899999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5899989999999999</c:v>
+                  <c:v>1.9999990000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7199970000000002</c:v>
+                  <c:v>4.6799980000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2399989999999992</c:v>
+                  <c:v>10.289998000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.119997000000001</c:v>
+                  <c:v>25.010003999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.269996999999996</c:v>
+                  <c:v>47.960003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.899994000000007</c:v>
+                  <c:v>94.650008999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153.73001099999999</c:v>
+                  <c:v>155.95002700000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>282.699951</c:v>
+                  <c:v>282.72000100000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>425.4599</c:v>
+                  <c:v>416.68997200000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>757.70989999999995</c:v>
+                  <c:v>754.37969999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1107.2700199999999</c:v>
+                  <c:v>1123.829956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1824.4102780000001</c:v>
+                  <c:v>1851.910034</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2733.3391109999998</c:v>
@@ -1977,43 +2020,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.86</c:v>
+                  <c:v>1.439999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2199990000000001</c:v>
+                  <c:v>3.919997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.55</c:v>
+                  <c:v>8.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.339995999999999</c:v>
+                  <c:v>23.789999000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.540000999999997</c:v>
+                  <c:v>67.049994999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158.29997299999999</c:v>
+                  <c:v>170.37994399999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>385.94003300000003</c:v>
+                  <c:v>398.43994099999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>886.61987299999998</c:v>
+                  <c:v>932.16009499999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2025.2098390000001</c:v>
+                  <c:v>2104.0402829999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4485.5703130000002</c:v>
+                  <c:v>4477.7304690000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10279.320313</c:v>
+                  <c:v>10384.141602</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22137.626952999999</c:v>
+                  <c:v>22621.693359000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47450.015625</c:v>
+                  <c:v>48435.164062999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>105516.484375</c:v>
@@ -2528,7 +2571,7 @@
             <c:numRef>
               <c:f>ford!$C$2:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2546,28 +2589,28 @@
                   <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0000000000000002E-5</c:v>
+                  <c:v>3.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4999999999999999E-4</c:v>
+                  <c:v>1.3999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1999999999999995E-4</c:v>
+                  <c:v>5.4000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.92E-3</c:v>
+                  <c:v>1.97E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1399999999999996E-3</c:v>
+                  <c:v>6.2100000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5909999999999999E-2</c:v>
+                  <c:v>2.3699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.2580000000000001E-2</c:v>
+                  <c:v>7.8329999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.28611999999999999</c:v>
+                  <c:v>0.27796999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.93942999999999999</c:v>
@@ -2785,7 +2828,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3088,43 +3131,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.67</c:v>
+                  <c:v>0.99999899999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5899989999999999</c:v>
+                  <c:v>1.9999990000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7199970000000002</c:v>
+                  <c:v>4.6799980000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2399989999999992</c:v>
+                  <c:v>10.289998000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.119997000000001</c:v>
+                  <c:v>25.010003999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.269996999999996</c:v>
+                  <c:v>47.960003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.899994000000007</c:v>
+                  <c:v>94.650008999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>153.73001099999999</c:v>
+                  <c:v>155.95002700000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>282.699951</c:v>
+                  <c:v>282.72000100000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>425.4599</c:v>
+                  <c:v>416.68997200000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>757.70989999999995</c:v>
+                  <c:v>754.37969999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1107.2700199999999</c:v>
+                  <c:v>1123.829956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1824.4102780000001</c:v>
+                  <c:v>1851.910034</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2733.3391109999998</c:v>
@@ -3562,6 +3605,22 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>glpk!$B$1:$Q$1</c:f>
@@ -4083,6 +4142,22 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>glpk!$B$1:$Q$1</c:f>
@@ -9390,8 +9465,8 @@
   <autoFilter ref="A1:D17" xr:uid="{BF7E861D-9DE2-40AD-88C0-6451C35A9101}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5B19A6E7-2110-48A5-86F2-766F4851F3A9}" name="i"/>
-    <tableColumn id="2" xr3:uid="{79CA9824-CC58-40BE-98E1-9EDA714D6AC6}" name=" flow" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{606F8269-695C-41BD-B27D-027E73869D8D}" name=" time" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{79CA9824-CC58-40BE-98E1-9EDA714D6AC6}" name=" flow" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{606F8269-695C-41BD-B27D-027E73869D8D}" name=" time"/>
     <tableColumn id="4" xr3:uid="{BECDD8F8-4382-4470-ADF4-EEE29F95643A}" name=" paths" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -9697,8 +9772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEF3413-4993-4967-8AB7-143E4D2D7BE1}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9706,7 +9781,7 @@
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -9728,13 +9803,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.86</v>
+        <v>1.439999</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0.67</v>
+        <v>0.99999899999999997</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9742,13 +9817,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2.2199990000000001</v>
+        <v>3.919997</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1.5899989999999999</v>
+        <v>1.9999990000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9756,13 +9831,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>5.55</v>
+        <v>8.93</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>3.7199970000000002</v>
+        <v>4.6799980000000003</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -9770,13 +9845,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>19.339995999999999</v>
+        <v>23.789999000000002</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>9.2399989999999992</v>
+        <v>10.289998000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -9784,13 +9859,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>54.540000999999997</v>
+        <v>67.049994999999996</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D6" s="1">
-        <v>23.119997000000001</v>
+        <v>25.010003999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9798,13 +9873,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>158.29997299999999</v>
+        <v>170.37994399999999</v>
       </c>
-      <c r="C7" s="2">
-        <v>5.0000000000000002E-5</v>
+      <c r="C7">
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="D7" s="1">
-        <v>48.269996999999996</v>
+        <v>47.960003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -9812,13 +9887,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>385.94003300000003</v>
+        <v>398.43994099999998</v>
       </c>
-      <c r="C8" s="2">
-        <v>1.4999999999999999E-4</v>
+      <c r="C8">
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="D8" s="1">
-        <v>96.899994000000007</v>
+        <v>94.650008999999997</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -9826,13 +9901,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>886.61987299999998</v>
+        <v>932.16009499999996</v>
       </c>
-      <c r="C9" s="2">
-        <v>5.1999999999999995E-4</v>
+      <c r="C9">
+        <v>5.4000000000000001E-4</v>
       </c>
       <c r="D9" s="1">
-        <v>153.73001099999999</v>
+        <v>155.95002700000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9840,13 +9915,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2025.2098390000001</v>
+        <v>2104.0402829999998</v>
       </c>
-      <c r="C10" s="2">
-        <v>1.92E-3</v>
+      <c r="C10">
+        <v>1.97E-3</v>
       </c>
       <c r="D10" s="1">
-        <v>282.699951</v>
+        <v>282.72000100000002</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9854,13 +9929,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>4485.5703130000002</v>
+        <v>4477.7304690000001</v>
       </c>
-      <c r="C11" s="2">
-        <v>6.1399999999999996E-3</v>
+      <c r="C11">
+        <v>6.2100000000000002E-3</v>
       </c>
       <c r="D11" s="1">
-        <v>425.4599</v>
+        <v>416.68997200000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -9868,13 +9943,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>10279.320313</v>
+        <v>10384.141602</v>
       </c>
-      <c r="C12" s="2">
-        <v>2.5909999999999999E-2</v>
+      <c r="C12">
+        <v>2.3699999999999999E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>757.70989999999995</v>
+        <v>754.37969999999996</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -9882,13 +9957,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>22137.626952999999</v>
+        <v>22621.693359000001</v>
       </c>
-      <c r="C13" s="2">
-        <v>8.2580000000000001E-2</v>
+      <c r="C13">
+        <v>7.8329999999999997E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>1107.2700199999999</v>
+        <v>1123.829956</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -9896,13 +9971,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>47450.015625</v>
+        <v>48435.164062999997</v>
       </c>
-      <c r="C14" s="2">
-        <v>0.28611999999999999</v>
+      <c r="C14">
+        <v>0.27796999999999999</v>
       </c>
       <c r="D14" s="1">
-        <v>1824.4102780000001</v>
+        <v>1851.910034</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -9912,7 +9987,7 @@
       <c r="B15" s="1">
         <v>105516.484375</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>0.93942999999999999</v>
       </c>
       <c r="D15" s="1">
@@ -9926,7 +10001,7 @@
       <c r="B16" s="1">
         <v>224130.953125</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>3.6695700000000002</v>
       </c>
       <c r="D16" s="1">
@@ -9940,7 +10015,7 @@
       <c r="B17" s="1">
         <v>473563.59375</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>17.220222</v>
       </c>
       <c r="D17" s="1">
@@ -9961,8 +10036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5CE0A7-8051-4005-A25D-DAB32C7FB51C}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
więcej fajniutkich wykresików mmmmmm
</commit_message>
<xml_diff>
--- a/5/1/res/res.xlsx
+++ b/5/1/res/res.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartor\IdeaProjects\aisd\5\1\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794923AE-32C6-4F4E-A7F7-7BA079FAB6C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288C61D0-2C5D-4507-BC0D-251873F607DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22860" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{19F8498E-A82F-437B-BA89-2E45E85CD9B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19F8498E-A82F-437B-BA89-2E45E85CD9B8}"/>
   </bookViews>
   <sheets>
     <sheet name="ford" sheetId="2" r:id="rId1"/>
     <sheet name="glpk" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">glpk!$A$1:$AY$63</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>k</t>
   </si>
@@ -50,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve"> paths</t>
+  </si>
+  <si>
+    <t>flow</t>
+  </si>
+  <si>
+    <t>time ms</t>
   </si>
 </sst>
 </file>
@@ -93,7 +102,10 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -279,22 +291,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -674,6 +670,555 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>glpk - 1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> example each - flow</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>glpk!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="lt1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4">
+                  <a:alpha val="70000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>glpk!$B$1:$Q$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>glpk!$B$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1245</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4192</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12227</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20559</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55291</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115185</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>234866</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>482930</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C4C-4055-BCE4-BB59643FFF19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="-20"/>
+        <c:axId val="505548360"/>
+        <c:axId val="505548688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="505548360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>input size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505548688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="505548688"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>flow</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505548360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -758,7 +1303,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> time</c:v>
+                  <c:v>time ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -836,23 +1381,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -917,52 +1445,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0000000000000001E-5</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-5</c:v>
+                  <c:v>3.0000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3999999999999999E-4</c:v>
+                  <c:v>0.13999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4000000000000001E-4</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.97E-3</c:v>
+                  <c:v>1.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.2100000000000002E-3</c:v>
+                  <c:v>6.21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3699999999999999E-2</c:v>
+                  <c:v>23.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.8329999999999997E-2</c:v>
+                  <c:v>78.33</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27796999999999999</c:v>
+                  <c:v>277.96999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.93942999999999999</c:v>
+                  <c:v>939.43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6695700000000002</c:v>
+                  <c:v>3669.57</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.220222</c:v>
+                  <c:v>17220.221999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,23 +1922,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>ford!$A$2:$A$17</c:f>
@@ -2432,7 +2943,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> time</c:v>
+                  <c:v>time ms</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2574,52 +3085,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0000000000000001E-5</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-5</c:v>
+                  <c:v>3.0000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3999999999999999E-4</c:v>
+                  <c:v>0.13999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4000000000000001E-4</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.97E-3</c:v>
+                  <c:v>1.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.2100000000000002E-3</c:v>
+                  <c:v>6.21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3699999999999999E-2</c:v>
+                  <c:v>23.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.8329999999999997E-2</c:v>
+                  <c:v>78.33</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27796999999999999</c:v>
+                  <c:v>277.96999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.93942999999999999</c:v>
+                  <c:v>939.43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6695700000000002</c:v>
+                  <c:v>3669.57</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.220222</c:v>
+                  <c:v>17220.221999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3491,8 +4002,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>glpk</a:t>
+              <a:t>glpk - 1 example each</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> - time</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3605,22 +4121,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>glpk!$B$1:$Q$1</c:f>
@@ -4027,9 +4527,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>glpk - log</a:t>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>glpk - 1 example each - time</a:t>
             </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4142,22 +4647,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:alpha val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>glpk!$B$1:$Q$1</c:f>
@@ -4546,7 +5035,611 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" cap="all" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>glpk - 1 example each - flow</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>glpk!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="lt1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4">
+                  <a:alpha val="70000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>glpk!$B$1:$Q$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>glpk!$B$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1245</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4192</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12227</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20559</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55291</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>115185</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>234866</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>482930</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0097-4453-9FAB-CFE2444AC08C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:overlap val="-20"/>
+        <c:axId val="505548360"/>
+        <c:axId val="505548688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="505548360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>input size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505548688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="505548688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>flow</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505548360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4866,6 +5959,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
@@ -5402,7 +6535,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5938,7 +7071,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6474,7 +7607,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7010,7 +8143,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7546,7 +8679,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8082,7 +9215,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8618,7 +9751,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9154,20 +10287,1092 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>614362</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>504826</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>211237</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>115575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9194,16 +11399,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>225525</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>96522</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9230,16 +11435,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>206474</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>91761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9266,16 +11471,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>235050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>120338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9304,16 +11509,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>119063</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>230288</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>91761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9342,16 +11547,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>185738</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>225525</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>120337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9385,16 +11590,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609598</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>215998</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>96525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9405,7 +11610,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -9421,16 +11628,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>225524</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>87000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9457,17 +11664,94 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>215999</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>91761</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6611A4DC-095F-401B-BD05-8833C43345DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>206475</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>96525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E4DCBE7-DB36-4EA6-BCC4-F3903C832AC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB10C286-77CE-4FD8-822C-8FAC2C950F09}" name="_100_windows_pcg" displayName="_100_windows_pcg" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17" xr:uid="{BF7E861D-9DE2-40AD-88C0-6451C35A9101}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BB10C286-77CE-4FD8-822C-8FAC2C950F09}" name="_100_windows_pcg" displayName="_100_windows_pcg" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{BF7E861D-9DE2-40AD-88C0-6451C35A9101}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5B19A6E7-2110-48A5-86F2-766F4851F3A9}" name="i"/>
-    <tableColumn id="2" xr3:uid="{79CA9824-CC58-40BE-98E1-9EDA714D6AC6}" name=" flow" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{606F8269-695C-41BD-B27D-027E73869D8D}" name=" time"/>
-    <tableColumn id="4" xr3:uid="{BECDD8F8-4382-4470-ADF4-EEE29F95643A}" name=" paths" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{79CA9824-CC58-40BE-98E1-9EDA714D6AC6}" name=" flow" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{606F8269-695C-41BD-B27D-027E73869D8D}" name="time ms" dataDxfId="0">
+      <calculatedColumnFormula>_100_windows_pcg[[#This Row],[ time]]*1000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BECDD8F8-4382-4470-ADF4-EEE29F95643A}" name=" paths" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{AA77E9FA-51B2-4C82-BCA6-EA7BD17F7E28}" name=" time"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9770,10 +12054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEF3413-4993-4967-8AB7-143E4D2D7BE1}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9784,7 +12068,7 @@
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -9792,13 +12076,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9806,13 +12093,17 @@
         <v>1.439999</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>1E-3</v>
       </c>
       <c r="D2" s="1">
         <v>0.99999899999999997</v>
       </c>
+      <c r="E2">
+        <v>9.9999999999999995E-7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9820,13 +12111,17 @@
         <v>3.919997</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>1E-3</v>
       </c>
       <c r="D3" s="1">
         <v>1.9999990000000001</v>
       </c>
+      <c r="E3">
+        <v>9.9999999999999995E-7</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9834,13 +12129,17 @@
         <v>8.93</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>2E-3</v>
       </c>
       <c r="D4" s="1">
         <v>4.6799980000000003</v>
       </c>
+      <c r="E4">
+        <v>1.9999999999999999E-6</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9848,13 +12147,17 @@
         <v>23.789999000000002</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D5" s="1">
         <v>10.289998000000001</v>
       </c>
+      <c r="E5">
+        <v>5.0000000000000004E-6</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9862,13 +12165,17 @@
         <v>67.049994999999996</v>
       </c>
       <c r="C6">
-        <v>1.0000000000000001E-5</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>0.01</v>
       </c>
       <c r="D6" s="1">
         <v>25.010003999999999</v>
       </c>
+      <c r="E6">
+        <v>1.0000000000000001E-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9876,13 +12183,17 @@
         <v>170.37994399999999</v>
       </c>
       <c r="C7">
-        <v>3.0000000000000001E-5</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="D7" s="1">
         <v>47.960003</v>
       </c>
+      <c r="E7">
+        <v>3.0000000000000001E-5</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9890,13 +12201,17 @@
         <v>398.43994099999998</v>
       </c>
       <c r="C8">
-        <v>1.3999999999999999E-4</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>0.13999999999999999</v>
       </c>
       <c r="D8" s="1">
         <v>94.650008999999997</v>
       </c>
+      <c r="E8">
+        <v>1.3999999999999999E-4</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9904,13 +12219,17 @@
         <v>932.16009499999996</v>
       </c>
       <c r="C9">
-        <v>5.4000000000000001E-4</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>0.54</v>
       </c>
       <c r="D9" s="1">
         <v>155.95002700000001</v>
       </c>
+      <c r="E9">
+        <v>5.4000000000000001E-4</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9918,13 +12237,17 @@
         <v>2104.0402829999998</v>
       </c>
       <c r="C10">
-        <v>1.97E-3</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>1.97</v>
       </c>
       <c r="D10" s="1">
         <v>282.72000100000002</v>
       </c>
+      <c r="E10">
+        <v>1.97E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9932,13 +12255,17 @@
         <v>4477.7304690000001</v>
       </c>
       <c r="C11">
-        <v>6.2100000000000002E-3</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>6.21</v>
       </c>
       <c r="D11" s="1">
         <v>416.68997200000001</v>
       </c>
+      <c r="E11">
+        <v>6.2100000000000002E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9946,13 +12273,17 @@
         <v>10384.141602</v>
       </c>
       <c r="C12">
-        <v>2.3699999999999999E-2</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>23.7</v>
       </c>
       <c r="D12" s="1">
         <v>754.37969999999996</v>
       </c>
+      <c r="E12">
+        <v>2.3699999999999999E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9960,13 +12291,17 @@
         <v>22621.693359000001</v>
       </c>
       <c r="C13">
-        <v>7.8329999999999997E-2</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>78.33</v>
       </c>
       <c r="D13" s="1">
         <v>1123.829956</v>
       </c>
+      <c r="E13">
+        <v>7.8329999999999997E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9974,13 +12309,17 @@
         <v>48435.164062999997</v>
       </c>
       <c r="C14">
-        <v>0.27796999999999999</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>277.96999999999997</v>
       </c>
       <c r="D14" s="1">
         <v>1851.910034</v>
       </c>
+      <c r="E14">
+        <v>0.27796999999999999</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9988,13 +12327,17 @@
         <v>105516.484375</v>
       </c>
       <c r="C15">
-        <v>0.93942999999999999</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>939.43</v>
       </c>
       <c r="D15" s="1">
         <v>2733.3391109999998</v>
       </c>
+      <c r="E15">
+        <v>0.93942999999999999</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10002,13 +12345,17 @@
         <v>224130.953125</v>
       </c>
       <c r="C16">
-        <v>3.6695700000000002</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>3669.57</v>
       </c>
       <c r="D16" s="1">
         <v>4417.7895509999998</v>
       </c>
+      <c r="E16">
+        <v>3.6695700000000002</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10016,10 +12363,14 @@
         <v>473563.59375</v>
       </c>
       <c r="C17">
-        <v>17.220222</v>
+        <f>_100_windows_pcg[[#This Row],[ time]]*1000</f>
+        <v>17220.221999999998</v>
       </c>
       <c r="D17" s="1">
         <v>6297.7001950000003</v>
+      </c>
+      <c r="E17">
+        <v>17.220222</v>
       </c>
     </row>
   </sheetData>
@@ -10034,10 +12385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5CE0A7-8051-4005-A25D-DAB32C7FB51C}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10148,9 +12499,63 @@
         <v>4575680.5999999996</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>144</v>
+      </c>
+      <c r="H3">
+        <v>498</v>
+      </c>
+      <c r="I3">
+        <v>960</v>
+      </c>
+      <c r="J3">
+        <v>1245</v>
+      </c>
+      <c r="K3">
+        <v>4192</v>
+      </c>
+      <c r="L3">
+        <v>12227</v>
+      </c>
+      <c r="M3">
+        <v>20559</v>
+      </c>
+      <c r="N3">
+        <v>55291</v>
+      </c>
+      <c r="O3">
+        <v>115185</v>
+      </c>
+      <c r="P3">
+        <v>234866</v>
+      </c>
+      <c r="Q3">
+        <v>482930</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>